<commit_message>
major excel changes and added codes to analize data when done
</commit_message>
<xml_diff>
--- a/Apple.xlsx
+++ b/Apple.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paula Yamada\OneDrive\Área de Trabalho\2021.2\cdados\cdados-projeto-1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alinsperedu-my.sharepoint.com/personal/carlosepy_al_insper_edu_br/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F2777D4-C2C4-420C-A6E5-C34ACF55656C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="8_{93509D0A-C4AA-4C11-AA86-F8B5168BC805}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B065B613-9636-4FAF-933F-98D066148C23}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="503">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="503">
   <si>
     <t>Treinamento</t>
   </si>
@@ -1772,7 +1772,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1807,6 +1807,14 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="ＭＳ Ｐゴシック"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1849,7 +1857,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1858,6 +1866,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -2199,8 +2208,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B301"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2213,7 +2222,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>502</v>
       </c>
     </row>
@@ -3415,309 +3424,459 @@
         <v>239</v>
       </c>
     </row>
-    <row r="241" spans="1:1">
+    <row r="241" spans="1:2">
       <c r="A241" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="242" spans="1:1">
+    <row r="242" spans="1:2">
       <c r="A242" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="243" spans="1:1">
+    <row r="243" spans="1:2">
       <c r="A243" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="244" spans="1:1">
+    <row r="244" spans="1:2">
       <c r="A244" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="245" spans="1:1">
+    <row r="245" spans="1:2">
       <c r="A245" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="246" spans="1:1">
+    <row r="246" spans="1:2">
       <c r="A246" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="247" spans="1:1">
+    <row r="247" spans="1:2">
       <c r="A247" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="248" spans="1:1">
+    <row r="248" spans="1:2">
       <c r="A248" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="249" spans="1:1">
+    <row r="249" spans="1:2">
       <c r="A249" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="250" spans="1:1">
+    <row r="250" spans="1:2">
       <c r="A250" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="251" spans="1:1">
+    <row r="251" spans="1:2">
       <c r="A251" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="252" spans="1:1">
+    <row r="252" spans="1:2">
       <c r="A252" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="253" spans="1:1">
+      <c r="B252">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2">
       <c r="A253" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="254" spans="1:1">
+      <c r="B253">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2">
       <c r="A254" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="255" spans="1:1">
+      <c r="B254">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2">
       <c r="A255" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="256" spans="1:1">
+      <c r="B255">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2">
       <c r="A256" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="257" spans="1:1">
+      <c r="B256">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2">
       <c r="A257" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="258" spans="1:1">
+      <c r="B257">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2">
       <c r="A258" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="259" spans="1:1">
+      <c r="B258">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2">
       <c r="A259" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="260" spans="1:1">
+      <c r="B259">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2">
       <c r="A260" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="261" spans="1:1">
+      <c r="B260">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2">
       <c r="A261" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="262" spans="1:1">
+      <c r="B261">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2">
       <c r="A262" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="263" spans="1:1">
+      <c r="B262">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2">
       <c r="A263" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="264" spans="1:1">
+      <c r="B263">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2">
       <c r="A264" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="265" spans="1:1">
+      <c r="B264">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2">
       <c r="A265" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="266" spans="1:1">
+      <c r="B265">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2">
       <c r="A266" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="267" spans="1:1">
+      <c r="B266">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2">
       <c r="A267" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="268" spans="1:1">
+      <c r="B267">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2">
       <c r="A268" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="269" spans="1:1">
+      <c r="B268">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2">
       <c r="A269" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="270" spans="1:1">
+      <c r="B269">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2">
       <c r="A270" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="271" spans="1:1">
+      <c r="B270">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2">
       <c r="A271" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="272" spans="1:1">
+      <c r="B271">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2">
       <c r="A272" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="273" spans="1:1">
+      <c r="B272">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2">
       <c r="A273" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="274" spans="1:1">
+      <c r="B273">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2">
       <c r="A274" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="275" spans="1:1">
+      <c r="B274">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2">
       <c r="A275" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="276" spans="1:1">
+      <c r="B275">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2">
       <c r="A276" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="277" spans="1:1">
+      <c r="B276">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2">
       <c r="A277" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="278" spans="1:1">
+      <c r="B277">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2">
       <c r="A278" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="279" spans="1:1">
+      <c r="B278">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2">
       <c r="A279" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="280" spans="1:1">
+      <c r="B279">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2">
       <c r="A280" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="281" spans="1:1">
+      <c r="B280">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2">
       <c r="A281" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="282" spans="1:1">
+      <c r="B281">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2">
       <c r="A282" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="283" spans="1:1">
+      <c r="B282">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2">
       <c r="A283" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="284" spans="1:1">
+      <c r="B283">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2">
       <c r="A284" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="285" spans="1:1">
+      <c r="B284">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2">
       <c r="A285" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="286" spans="1:1">
+      <c r="B285">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2">
       <c r="A286" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="287" spans="1:1">
+      <c r="B286">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2">
       <c r="A287" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="288" spans="1:1">
+      <c r="B287">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2">
       <c r="A288" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="289" spans="1:1">
+      <c r="B288">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2">
       <c r="A289" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="290" spans="1:1" ht="15">
+      <c r="B289">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2" ht="15">
       <c r="A290" s="2" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="291" spans="1:1">
+      <c r="B290">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="291" spans="1:2">
       <c r="A291" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="292" spans="1:1">
+      <c r="B291">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="292" spans="1:2">
       <c r="A292" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="293" spans="1:1" ht="15">
+      <c r="B292">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2" ht="15">
       <c r="A293" s="2" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="294" spans="1:1">
+      <c r="B293">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="294" spans="1:2">
       <c r="A294" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="295" spans="1:1">
+      <c r="B294">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="295" spans="1:2">
       <c r="A295" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="296" spans="1:1">
+      <c r="B295">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2">
       <c r="A296" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="297" spans="1:1">
+      <c r="B296">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="297" spans="1:2">
       <c r="A297" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="298" spans="1:1">
+      <c r="B297">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="298" spans="1:2">
       <c r="A298" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="299" spans="1:1">
+      <c r="B298">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="299" spans="1:2">
       <c r="A299" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="300" spans="1:1">
+      <c r="B299">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="300" spans="1:2">
       <c r="A300" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="301" spans="1:1">
+      <c r="B300">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="301" spans="1:2">
       <c r="A301" t="s">
         <v>300</v>
+      </c>
+      <c r="B301">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3733,1021 +3892,1872 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:A201"/>
+  <dimension ref="A1:E201"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
+  <cols>
+    <col min="2" max="2" width="13.75" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
+      <c r="B1" s="3" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="3" spans="1:1">
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="4" spans="1:1">
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="5" spans="1:1">
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="6" spans="1:1">
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="7" spans="1:1">
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="8" spans="1:1">
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="9" spans="1:1">
+      <c r="B8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="10" spans="1:1">
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="11" spans="1:1">
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="12" spans="1:1">
+      <c r="B11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="13" spans="1:1">
+      <c r="B12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="14" spans="1:1">
+      <c r="B13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="15" spans="1:1">
+      <c r="B14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="16" spans="1:1">
+      <c r="B15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="17" spans="1:1">
+      <c r="B16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="18" spans="1:1">
+      <c r="B17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="19" spans="1:1">
+      <c r="B18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="20" spans="1:1">
+      <c r="B19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
       <c r="A20" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="21" spans="1:1">
+      <c r="B20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
       <c r="A21" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="22" spans="1:1">
+      <c r="B21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
       <c r="A22" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="23" spans="1:1">
+      <c r="B22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
       <c r="A23" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="24" spans="1:1">
+      <c r="B23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
       <c r="A24" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="25" spans="1:1">
+      <c r="B24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
       <c r="A25" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="26" spans="1:1">
+      <c r="B25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
       <c r="A26" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="27" spans="1:1">
+      <c r="B26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
       <c r="A27" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="28" spans="1:1">
+      <c r="B27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
       <c r="A28" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="29" spans="1:1">
+      <c r="B28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
       <c r="A29" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="30" spans="1:1">
+      <c r="B29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
       <c r="A30" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="31" spans="1:1">
+      <c r="B30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
       <c r="A31" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="32" spans="1:1">
+      <c r="B31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
       <c r="A32" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="33" spans="1:1">
+      <c r="B32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
       <c r="A33" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="34" spans="1:1">
+      <c r="B33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
       <c r="A34" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="35" spans="1:1">
+      <c r="B34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
       <c r="A35" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="36" spans="1:1">
+      <c r="B35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
       <c r="A36" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="37" spans="1:1">
+      <c r="B36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
       <c r="A37" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="38" spans="1:1">
+      <c r="B37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
       <c r="A38" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="39" spans="1:1">
+      <c r="B38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
       <c r="A39" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="40" spans="1:1">
+      <c r="B39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
       <c r="A40" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="41" spans="1:1">
+      <c r="B40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
       <c r="A41" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="42" spans="1:1">
+      <c r="B41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
       <c r="A42" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="43" spans="1:1">
+      <c r="B42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
       <c r="A43" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="44" spans="1:1">
+      <c r="B43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
       <c r="A44" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="45" spans="1:1">
+      <c r="B44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
       <c r="A45" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="46" spans="1:1">
+      <c r="B45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
       <c r="A46" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="47" spans="1:1">
+      <c r="B46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
       <c r="A47" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="48" spans="1:1">
+      <c r="B47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
       <c r="A48" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="49" spans="1:1">
+      <c r="B48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
       <c r="A49" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="50" spans="1:1">
+      <c r="B49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
       <c r="A50" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="51" spans="1:1">
+      <c r="B50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
       <c r="A51" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="52" spans="1:1">
+      <c r="B51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
       <c r="A52" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="53" spans="1:1">
+      <c r="B52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
       <c r="A53" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="54" spans="1:1">
+      <c r="B53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
       <c r="A54" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="55" spans="1:1">
+      <c r="B54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
       <c r="A55" t="s">
         <v>355</v>
       </c>
-    </row>
-    <row r="56" spans="1:1">
+      <c r="B55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
       <c r="A56" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="57" spans="1:1">
+      <c r="B56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
       <c r="A57" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="58" spans="1:1">
+      <c r="B57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
       <c r="A58" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="59" spans="1:1">
+      <c r="B58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
       <c r="A59" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="60" spans="1:1">
+      <c r="B59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
       <c r="A60" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="61" spans="1:1">
+      <c r="B60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
       <c r="A61" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="62" spans="1:1">
+      <c r="B61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
       <c r="A62" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="63" spans="1:1">
+      <c r="B62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
       <c r="A63" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="64" spans="1:1">
+      <c r="B63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
       <c r="A64" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="65" spans="1:1">
+      <c r="B64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
       <c r="A65" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="66" spans="1:1">
+      <c r="B65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
       <c r="A66" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="67" spans="1:1">
+      <c r="B66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
       <c r="A67" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="68" spans="1:1">
+      <c r="B67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
       <c r="A68" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="69" spans="1:1">
+      <c r="B68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
       <c r="A69" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="70" spans="1:1">
+      <c r="B69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
       <c r="A70" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="71" spans="1:1">
+      <c r="B70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
       <c r="A71" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="72" spans="1:1">
+      <c r="B71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
       <c r="A72" t="s">
         <v>372</v>
       </c>
-    </row>
-    <row r="73" spans="1:1">
+      <c r="B72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
       <c r="A73" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="74" spans="1:1">
+      <c r="B73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
       <c r="A74" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="75" spans="1:1">
+      <c r="B74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
       <c r="A75" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="76" spans="1:1">
+      <c r="B75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
       <c r="A76" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="77" spans="1:1">
+      <c r="B76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
       <c r="A77" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="78" spans="1:1">
+      <c r="B77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
       <c r="A78" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="79" spans="1:1">
+      <c r="B78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
       <c r="A79" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="80" spans="1:1">
+      <c r="B79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
       <c r="A80" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="81" spans="1:1">
+      <c r="B80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
       <c r="A81" t="s">
         <v>381</v>
       </c>
-    </row>
-    <row r="82" spans="1:1">
+      <c r="B81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
       <c r="A82" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="83" spans="1:1">
+      <c r="B82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
       <c r="A83" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="84" spans="1:1">
+      <c r="B83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
       <c r="A84" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="85" spans="1:1">
+      <c r="B84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
       <c r="A85" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="86" spans="1:1">
+      <c r="B85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
       <c r="A86" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="87" spans="1:1">
+      <c r="B86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
       <c r="A87" t="s">
         <v>387</v>
       </c>
-    </row>
-    <row r="88" spans="1:1">
+      <c r="B87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
       <c r="A88" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="89" spans="1:1">
+      <c r="B88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
       <c r="A89" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="90" spans="1:1">
+      <c r="B89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
       <c r="A90" t="s">
         <v>390</v>
       </c>
-    </row>
-    <row r="91" spans="1:1">
+      <c r="B90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
       <c r="A91" t="s">
         <v>391</v>
       </c>
-    </row>
-    <row r="92" spans="1:1">
+      <c r="B91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
       <c r="A92" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="93" spans="1:1">
+      <c r="B92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
       <c r="A93" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="94" spans="1:1">
+      <c r="B93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
       <c r="A94" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="95" spans="1:1">
+      <c r="B94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
       <c r="A95" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="96" spans="1:1">
+      <c r="B95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
       <c r="A96" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="97" spans="1:1">
+      <c r="B96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
       <c r="A97" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="98" spans="1:1">
+      <c r="B97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
       <c r="A98" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="99" spans="1:1">
+      <c r="B98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
       <c r="A99" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="100" spans="1:1">
+      <c r="B99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
       <c r="A100" t="s">
         <v>400</v>
       </c>
-    </row>
-    <row r="101" spans="1:1">
+      <c r="B100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
       <c r="A101" t="s">
         <v>401</v>
       </c>
-    </row>
-    <row r="102" spans="1:1">
+      <c r="B101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
       <c r="A102" t="s">
         <v>402</v>
       </c>
-    </row>
-    <row r="103" spans="1:1">
+      <c r="B102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
       <c r="A103" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="104" spans="1:1">
+      <c r="B103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
       <c r="A104" t="s">
         <v>404</v>
       </c>
-    </row>
-    <row r="105" spans="1:1">
+      <c r="B104">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
       <c r="A105" t="s">
         <v>405</v>
       </c>
-    </row>
-    <row r="106" spans="1:1">
+      <c r="B105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
       <c r="A106" t="s">
         <v>406</v>
       </c>
-    </row>
-    <row r="107" spans="1:1">
+      <c r="B106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
       <c r="A107" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="108" spans="1:1">
+      <c r="B107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
       <c r="A108" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="109" spans="1:1">
+      <c r="B108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
       <c r="A109" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="110" spans="1:1">
+      <c r="B109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2">
       <c r="A110" t="s">
         <v>410</v>
       </c>
-    </row>
-    <row r="111" spans="1:1">
+      <c r="B110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
       <c r="A111" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="112" spans="1:1">
+      <c r="B111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2">
       <c r="A112" t="s">
         <v>412</v>
       </c>
-    </row>
-    <row r="113" spans="1:1">
+      <c r="B112">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2">
       <c r="A113" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="114" spans="1:1">
+      <c r="B113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
       <c r="A114" t="s">
         <v>414</v>
       </c>
-    </row>
-    <row r="115" spans="1:1">
+      <c r="B114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2">
       <c r="A115" t="s">
         <v>415</v>
       </c>
-    </row>
-    <row r="116" spans="1:1">
+      <c r="B115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2">
       <c r="A116" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="117" spans="1:1">
+      <c r="B116">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2">
       <c r="A117" t="s">
         <v>417</v>
       </c>
-    </row>
-    <row r="118" spans="1:1">
+      <c r="B117">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2">
       <c r="A118" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="119" spans="1:1">
+      <c r="B118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2">
       <c r="A119" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="120" spans="1:1">
+      <c r="B119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2">
       <c r="A120" t="s">
         <v>420</v>
       </c>
-    </row>
-    <row r="121" spans="1:1">
+      <c r="B120">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2">
       <c r="A121" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="122" spans="1:1">
+      <c r="B121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2">
       <c r="A122" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="123" spans="1:1">
+      <c r="B122">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2">
       <c r="A123" t="s">
         <v>423</v>
       </c>
-    </row>
-    <row r="124" spans="1:1">
+      <c r="B123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2">
       <c r="A124" t="s">
         <v>424</v>
       </c>
-    </row>
-    <row r="125" spans="1:1">
+      <c r="B124">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2">
       <c r="A125" t="s">
         <v>425</v>
       </c>
-    </row>
-    <row r="126" spans="1:1">
+      <c r="B125">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2">
       <c r="A126" t="s">
         <v>426</v>
       </c>
-    </row>
-    <row r="127" spans="1:1">
+      <c r="B126">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2">
       <c r="A127" t="s">
         <v>427</v>
       </c>
-    </row>
-    <row r="128" spans="1:1">
+      <c r="B127">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2">
       <c r="A128" t="s">
         <v>428</v>
       </c>
-    </row>
-    <row r="129" spans="1:1">
+      <c r="B128">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2">
       <c r="A129" t="s">
         <v>429</v>
       </c>
-    </row>
-    <row r="130" spans="1:1">
+      <c r="B129">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2">
       <c r="A130" t="s">
         <v>430</v>
       </c>
-    </row>
-    <row r="131" spans="1:1">
+      <c r="B130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2">
       <c r="A131" t="s">
         <v>431</v>
       </c>
-    </row>
-    <row r="132" spans="1:1">
+      <c r="B131">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2">
       <c r="A132" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="133" spans="1:1">
+      <c r="B132">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2">
       <c r="A133" t="s">
         <v>433</v>
       </c>
-    </row>
-    <row r="134" spans="1:1">
+      <c r="B133">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2">
       <c r="A134" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="135" spans="1:1">
+      <c r="B134">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2">
       <c r="A135" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="136" spans="1:1">
+      <c r="B135">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2">
       <c r="A136" t="s">
         <v>436</v>
       </c>
-    </row>
-    <row r="137" spans="1:1">
+      <c r="B136">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2">
       <c r="A137" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="138" spans="1:1">
+      <c r="B137">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2">
       <c r="A138" t="s">
         <v>438</v>
       </c>
-    </row>
-    <row r="139" spans="1:1">
+      <c r="B138">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2">
       <c r="A139" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="140" spans="1:1">
+      <c r="B139">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2">
       <c r="A140" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="141" spans="1:1">
+      <c r="B140">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2">
       <c r="A141" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="142" spans="1:1">
+      <c r="B141">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2">
       <c r="A142" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="143" spans="1:1">
+      <c r="B142">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2">
       <c r="A143" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="144" spans="1:1">
+      <c r="B143">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2">
       <c r="A144" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="145" spans="1:1">
+      <c r="B144">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2">
       <c r="A145" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="146" spans="1:1">
+      <c r="B145">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2">
       <c r="A146" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="147" spans="1:1">
+      <c r="B146">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2">
       <c r="A147" t="s">
         <v>447</v>
       </c>
-    </row>
-    <row r="148" spans="1:1">
+      <c r="B147">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2">
       <c r="A148" t="s">
         <v>448</v>
       </c>
-    </row>
-    <row r="149" spans="1:1">
+      <c r="B148">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2">
       <c r="A149" t="s">
         <v>449</v>
       </c>
-    </row>
-    <row r="150" spans="1:1">
+      <c r="B149">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2">
       <c r="A150" t="s">
         <v>450</v>
       </c>
-    </row>
-    <row r="151" spans="1:1">
+      <c r="B150">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2">
       <c r="A151" t="s">
         <v>451</v>
       </c>
-    </row>
-    <row r="152" spans="1:1">
+      <c r="B151">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2">
       <c r="A152" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="153" spans="1:1">
+      <c r="B152">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2">
       <c r="A153" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="154" spans="1:1">
+      <c r="B153">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2">
       <c r="A154" t="s">
         <v>454</v>
       </c>
-    </row>
-    <row r="155" spans="1:1">
+      <c r="B154">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2">
       <c r="A155" t="s">
         <v>455</v>
       </c>
-    </row>
-    <row r="156" spans="1:1">
+      <c r="B155">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2">
       <c r="A156" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="157" spans="1:1">
+      <c r="B156">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2">
       <c r="A157" t="s">
         <v>457</v>
       </c>
-    </row>
-    <row r="158" spans="1:1">
+      <c r="B157">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2">
       <c r="A158" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="159" spans="1:1">
+      <c r="B158">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2">
       <c r="A159" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="160" spans="1:1">
+      <c r="B159">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2">
       <c r="A160" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="161" spans="1:1">
+      <c r="B160">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2">
       <c r="A161" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="162" spans="1:1">
+      <c r="B161">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2">
       <c r="A162" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="163" spans="1:1">
+      <c r="B162">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2">
       <c r="A163" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="164" spans="1:1">
+      <c r="B163">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2">
       <c r="A164" t="s">
         <v>464</v>
       </c>
-    </row>
-    <row r="165" spans="1:1">
+      <c r="B164">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2">
       <c r="A165" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="166" spans="1:1">
+      <c r="B165">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2">
       <c r="A166" t="s">
         <v>466</v>
       </c>
-    </row>
-    <row r="167" spans="1:1">
+      <c r="B166">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2">
       <c r="A167" t="s">
         <v>467</v>
       </c>
-    </row>
-    <row r="168" spans="1:1">
+      <c r="B167">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2">
       <c r="A168" t="s">
         <v>468</v>
       </c>
-    </row>
-    <row r="169" spans="1:1">
+      <c r="B168">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2">
       <c r="A169" t="s">
         <v>469</v>
       </c>
-    </row>
-    <row r="170" spans="1:1">
+      <c r="B169">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2">
       <c r="A170" t="s">
         <v>470</v>
       </c>
-    </row>
-    <row r="171" spans="1:1">
+      <c r="B170">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2">
       <c r="A171" t="s">
         <v>471</v>
       </c>
-    </row>
-    <row r="172" spans="1:1">
+      <c r="B171">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2">
       <c r="A172" t="s">
         <v>472</v>
       </c>
-    </row>
-    <row r="173" spans="1:1">
+      <c r="B172">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2">
       <c r="A173" t="s">
         <v>473</v>
       </c>
-    </row>
-    <row r="174" spans="1:1">
+      <c r="B173">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2">
       <c r="A174" t="s">
         <v>474</v>
       </c>
-    </row>
-    <row r="175" spans="1:1">
+      <c r="B174">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2">
       <c r="A175" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="176" spans="1:1">
+      <c r="B175">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2">
       <c r="A176" t="s">
         <v>476</v>
       </c>
-    </row>
-    <row r="177" spans="1:1">
+      <c r="B176">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2">
       <c r="A177" t="s">
         <v>477</v>
       </c>
-    </row>
-    <row r="178" spans="1:1">
+      <c r="B177">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2">
       <c r="A178" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="179" spans="1:1">
+      <c r="B178">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2">
       <c r="A179" t="s">
         <v>479</v>
       </c>
-    </row>
-    <row r="180" spans="1:1">
+      <c r="B179">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2">
       <c r="A180" t="s">
         <v>480</v>
       </c>
-    </row>
-    <row r="181" spans="1:1">
+      <c r="B180">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2">
       <c r="A181" t="s">
         <v>481</v>
       </c>
-    </row>
-    <row r="182" spans="1:1">
+      <c r="B181">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2">
       <c r="A182" t="s">
         <v>482</v>
       </c>
-    </row>
-    <row r="183" spans="1:1">
+      <c r="B182">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2">
       <c r="A183" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="184" spans="1:1">
+      <c r="B183">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2">
       <c r="A184" t="s">
         <v>484</v>
       </c>
-    </row>
-    <row r="185" spans="1:1">
+      <c r="B184">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2">
       <c r="A185" t="s">
         <v>485</v>
       </c>
-    </row>
-    <row r="186" spans="1:1">
+      <c r="B185">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2">
       <c r="A186" t="s">
         <v>486</v>
       </c>
-    </row>
-    <row r="187" spans="1:1">
+      <c r="B186">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2">
       <c r="A187" t="s">
         <v>487</v>
       </c>
-    </row>
-    <row r="188" spans="1:1">
+      <c r="B187">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2">
       <c r="A188" t="s">
         <v>488</v>
       </c>
-    </row>
-    <row r="189" spans="1:1">
+      <c r="B188">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2">
       <c r="A189" t="s">
         <v>489</v>
       </c>
-    </row>
-    <row r="190" spans="1:1">
+      <c r="B189">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2">
       <c r="A190" t="s">
         <v>490</v>
       </c>
-    </row>
-    <row r="191" spans="1:1">
+      <c r="B190">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2">
       <c r="A191" t="s">
         <v>491</v>
       </c>
-    </row>
-    <row r="192" spans="1:1">
+      <c r="B191">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2">
       <c r="A192" t="s">
         <v>492</v>
       </c>
-    </row>
-    <row r="193" spans="1:1">
+      <c r="B192">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2">
       <c r="A193" t="s">
         <v>493</v>
       </c>
-    </row>
-    <row r="194" spans="1:1">
+      <c r="B193">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2">
       <c r="A194" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="195" spans="1:1">
+      <c r="B194">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2">
       <c r="A195" t="s">
         <v>495</v>
       </c>
-    </row>
-    <row r="196" spans="1:1">
+      <c r="B195">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2">
       <c r="A196" t="s">
         <v>496</v>
       </c>
-    </row>
-    <row r="197" spans="1:1">
+      <c r="B196">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2">
       <c r="A197" t="s">
         <v>497</v>
       </c>
-    </row>
-    <row r="198" spans="1:1">
+      <c r="B197">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2">
       <c r="A198" t="s">
         <v>498</v>
       </c>
-    </row>
-    <row r="199" spans="1:1">
+      <c r="B198">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2">
       <c r="A199" t="s">
         <v>499</v>
       </c>
-    </row>
-    <row r="200" spans="1:1">
+      <c r="B199">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2">
       <c r="A200" t="s">
         <v>500</v>
       </c>
-    </row>
-    <row r="201" spans="1:1">
+      <c r="B200">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2">
       <c r="A201" t="s">
         <v>501</v>
+      </c>
+      <c r="B201">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C3E9AF5A3A25204D946F822282C6A3FA" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="10847e6e73796df1c5199be7b9d9bbac">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="760d57ad-6986-40cd-8f44-ffd131bfd400" xmlns:ns4="f201cd4c-f14b-4b50-a959-57fff54ecbfb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="472fd269b72ff4a8b63318727dbe4b51" ns3:_="" ns4:_="">
+    <xsd:import namespace="760d57ad-6986-40cd-8f44-ffd131bfd400"/>
+    <xsd:import namespace="f201cd4c-f14b-4b50-a959-57fff54ecbfb"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns4:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns4:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns4:SharingHintHash" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="760d57ad-6986-40cd-8f44-ffd131bfd400" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="10" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="11" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="f201cd4c-f14b-4b50-a959-57fff54ecbfb" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="12" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="13" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="SharingHintHash" ma:index="14" nillable="true" ma:displayName="Sharing Hint Hash" ma:hidden="true" ma:internalName="SharingHintHash" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{42369E42-EB33-4F40-8133-C30C1A69E39F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="760d57ad-6986-40cd-8f44-ffd131bfd400"/>
+    <ds:schemaRef ds:uri="f201cd4c-f14b-4b50-a959-57fff54ecbfb"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D5B91BB-EA3D-4631-B192-ED1BCC344988}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74C81C81-D3B0-4785-8AEB-71C808FAD019}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="760d57ad-6986-40cd-8f44-ffd131bfd400"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="f201cd4c-f14b-4b50-a959-57fff54ecbfb"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Classificação de mais tweets
</commit_message>
<xml_diff>
--- a/Apple.xlsx
+++ b/Apple.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alinsperedu-my.sharepoint.com/personal/carlosepy_al_insper_edu_br/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjcpe\OneDrive\Área de Trabalho\C.Dados\Projeto 1\cdados-projeto-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{93509D0A-C4AA-4C11-AA86-F8B5168BC805}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B065B613-9636-4FAF-933F-98D066148C23}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3819CB2-C358-4DE3-BC57-454137BC7709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
@@ -1776,7 +1776,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1784,7 +1784,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1797,7 +1797,7 @@
     </font>
     <font>
       <sz val="6"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -1806,14 +1806,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2208,14 +2208,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B301"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="63" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="13.125" customWidth="1"/>
-    <col min="2" max="2" width="13.875" customWidth="1"/>
+    <col min="1" max="1" width="255.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -2238,1246 +2238,1993 @@
       <c r="A3" t="s">
         <v>2</v>
       </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>13</v>
       </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1">
+      <c r="B16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1">
+      <c r="B17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1">
+      <c r="B18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1">
+      <c r="B19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
       <c r="A20" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1">
+      <c r="B20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
       <c r="A21" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:1">
+      <c r="B21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
       <c r="A22" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:1">
+      <c r="B22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
       <c r="A23" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:1">
+      <c r="B23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
       <c r="A24" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:1">
+      <c r="B24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
       <c r="A25" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:1">
+      <c r="B25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
       <c r="A26" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:1">
+      <c r="B26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
       <c r="A27" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:1">
+      <c r="B27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
       <c r="A28" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:1">
+      <c r="B28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
       <c r="A29" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:1">
+      <c r="B29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
       <c r="A30" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:1">
+      <c r="B30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
       <c r="A31" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:1">
+      <c r="B31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
       <c r="A32" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:1">
+      <c r="B32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
       <c r="A33" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:1">
+      <c r="B33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
       <c r="A34" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:1">
+      <c r="B34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
       <c r="A35" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:1">
+      <c r="B35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
       <c r="A36" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:1">
+      <c r="B36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
       <c r="A37" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:1">
+      <c r="B37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
       <c r="A38" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="1:1">
+      <c r="B38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
       <c r="A39" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="40" spans="1:1">
+      <c r="B39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
       <c r="A40" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="41" spans="1:1">
+      <c r="B40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
       <c r="A41" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="42" spans="1:1">
+      <c r="B41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
       <c r="A42" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="43" spans="1:1">
+      <c r="B42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
       <c r="A43" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="44" spans="1:1">
+      <c r="B43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
       <c r="A44" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="45" spans="1:1">
+      <c r="B44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
       <c r="A45" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="46" spans="1:1">
+      <c r="B45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
       <c r="A46" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="47" spans="1:1">
+      <c r="B46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
       <c r="A47" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="48" spans="1:1">
+      <c r="B47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
       <c r="A48" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="49" spans="1:1">
+      <c r="B48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
       <c r="A49" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="50" spans="1:1">
+      <c r="B49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
       <c r="A50" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="51" spans="1:1">
+      <c r="B50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
       <c r="A51" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="52" spans="1:1">
+      <c r="B51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
       <c r="A52" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="53" spans="1:1">
+      <c r="B52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
       <c r="A53" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="54" spans="1:1">
+      <c r="B53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
       <c r="A54" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="55" spans="1:1">
+      <c r="B54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
       <c r="A55" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="56" spans="1:1">
+      <c r="B55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
       <c r="A56" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="57" spans="1:1">
+      <c r="B56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
       <c r="A57" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="58" spans="1:1">
+      <c r="B57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
       <c r="A58" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="59" spans="1:1">
+      <c r="B58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
       <c r="A59" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="60" spans="1:1">
+      <c r="B59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
       <c r="A60" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="61" spans="1:1">
+      <c r="B60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
       <c r="A61" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="62" spans="1:1">
+      <c r="B61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
       <c r="A62" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="63" spans="1:1">
+      <c r="B62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
       <c r="A63" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="64" spans="1:1">
+      <c r="B63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
       <c r="A64" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="65" spans="1:1">
+      <c r="B64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
       <c r="A65" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="66" spans="1:1">
+      <c r="B65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
       <c r="A66" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="67" spans="1:1">
+      <c r="B66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
       <c r="A67" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="68" spans="1:1">
+      <c r="B67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
       <c r="A68" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="69" spans="1:1">
+      <c r="B68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
       <c r="A69" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="70" spans="1:1">
+      <c r="B69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
       <c r="A70" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="71" spans="1:1">
+      <c r="B70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
       <c r="A71" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="72" spans="1:1">
+      <c r="B71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
       <c r="A72" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="73" spans="1:1">
+      <c r="B72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
       <c r="A73" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="74" spans="1:1">
+      <c r="B73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
       <c r="A74" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="75" spans="1:1">
+      <c r="B74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
       <c r="A75" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="76" spans="1:1">
+      <c r="B75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
       <c r="A76" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="77" spans="1:1">
+      <c r="B76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
       <c r="A77" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="78" spans="1:1">
+      <c r="B77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
       <c r="A78" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="79" spans="1:1">
+      <c r="B78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
       <c r="A79" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="80" spans="1:1">
+      <c r="B79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
       <c r="A80" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="81" spans="1:1">
+      <c r="B80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
       <c r="A81" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="82" spans="1:1">
+      <c r="B81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
       <c r="A82" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="83" spans="1:1">
+      <c r="B82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
       <c r="A83" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="84" spans="1:1">
+      <c r="B83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
       <c r="A84" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="85" spans="1:1">
+      <c r="B84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
       <c r="A85" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="86" spans="1:1">
+      <c r="B85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
       <c r="A86" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="87" spans="1:1">
+      <c r="B86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
       <c r="A87" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="88" spans="1:1">
+      <c r="B87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
       <c r="A88" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="89" spans="1:1">
+      <c r="B88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
       <c r="A89" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="90" spans="1:1">
+      <c r="B89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
       <c r="A90" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="91" spans="1:1">
+      <c r="B90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
       <c r="A91" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="92" spans="1:1">
+      <c r="B91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
       <c r="A92" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="93" spans="1:1">
+      <c r="B92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
       <c r="A93" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="94" spans="1:1">
+      <c r="B93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
       <c r="A94" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="95" spans="1:1">
+      <c r="B94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
       <c r="A95" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="96" spans="1:1">
+      <c r="B95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
       <c r="A96" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="97" spans="1:1">
+      <c r="B96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
       <c r="A97" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="98" spans="1:1">
+      <c r="B97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
       <c r="A98" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="99" spans="1:1">
+      <c r="B98">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
       <c r="A99" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="100" spans="1:1">
+      <c r="B99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
       <c r="A100" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="101" spans="1:1">
+      <c r="B100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
       <c r="A101" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="102" spans="1:1">
+      <c r="B101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
       <c r="A102" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="103" spans="1:1">
+      <c r="B102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
       <c r="A103" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="104" spans="1:1">
+      <c r="B103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
       <c r="A104" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="105" spans="1:1">
+      <c r="B104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
       <c r="A105" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="106" spans="1:1">
+      <c r="B105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
       <c r="A106" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="107" spans="1:1">
+      <c r="B106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
       <c r="A107" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="108" spans="1:1">
+      <c r="B107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
       <c r="A108" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="109" spans="1:1">
+      <c r="B108">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
       <c r="A109" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="110" spans="1:1">
+      <c r="B109">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2">
       <c r="A110" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="111" spans="1:1">
+      <c r="B110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
       <c r="A111" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="112" spans="1:1">
+      <c r="B111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2">
       <c r="A112" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="113" spans="1:1">
+      <c r="B112">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2">
       <c r="A113" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="114" spans="1:1">
+      <c r="B113">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
       <c r="A114" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="115" spans="1:1">
+      <c r="B114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2">
       <c r="A115" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="116" spans="1:1">
+      <c r="B115">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2">
       <c r="A116" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="117" spans="1:1">
+      <c r="B116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2">
       <c r="A117" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="118" spans="1:1">
+      <c r="B117">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2">
       <c r="A118" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="119" spans="1:1">
+      <c r="B118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2">
       <c r="A119" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="120" spans="1:1">
+      <c r="B119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2">
       <c r="A120" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="121" spans="1:1">
+      <c r="B120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2">
       <c r="A121" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="122" spans="1:1">
+      <c r="B121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2">
       <c r="A122" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="123" spans="1:1">
+      <c r="B122">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2">
       <c r="A123" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="124" spans="1:1">
+      <c r="B123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2">
       <c r="A124" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="125" spans="1:1">
+      <c r="B124">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2">
       <c r="A125" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="126" spans="1:1">
+      <c r="B125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2">
       <c r="A126" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="127" spans="1:1">
+      <c r="B126">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2">
       <c r="A127" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="128" spans="1:1">
+      <c r="B127">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2">
       <c r="A128" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="129" spans="1:1">
+      <c r="B128">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2">
       <c r="A129" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="130" spans="1:1">
+      <c r="B129">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2">
       <c r="A130" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="131" spans="1:1">
+      <c r="B130">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2">
       <c r="A131" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="132" spans="1:1">
+      <c r="B131">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2">
       <c r="A132" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="133" spans="1:1">
+      <c r="B132">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2">
       <c r="A133" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="134" spans="1:1">
+      <c r="B133">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2">
       <c r="A134" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="135" spans="1:1">
+      <c r="B134">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2">
       <c r="A135" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="136" spans="1:1">
+      <c r="B135">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2">
       <c r="A136" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="137" spans="1:1">
+      <c r="B136">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2">
       <c r="A137" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="138" spans="1:1">
+      <c r="B137">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2">
       <c r="A138" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="139" spans="1:1">
+      <c r="B138">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2">
       <c r="A139" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="140" spans="1:1">
+      <c r="B139">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2">
       <c r="A140" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="141" spans="1:1">
+      <c r="B140">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2">
       <c r="A141" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="142" spans="1:1">
+      <c r="B141">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2">
       <c r="A142" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="143" spans="1:1">
+      <c r="B142">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2">
       <c r="A143" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="144" spans="1:1">
+      <c r="B143">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2">
       <c r="A144" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="145" spans="1:1">
+      <c r="B144">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2">
       <c r="A145" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="146" spans="1:1">
+      <c r="B145">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2">
       <c r="A146" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="147" spans="1:1">
+      <c r="B146">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2">
       <c r="A147" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="148" spans="1:1">
+      <c r="B147">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2">
       <c r="A148" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="149" spans="1:1">
+      <c r="B148">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2">
       <c r="A149" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="150" spans="1:1">
+      <c r="B149">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2">
       <c r="A150" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="151" spans="1:1">
+      <c r="B150">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2">
       <c r="A151" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="152" spans="1:1">
+      <c r="B151">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2">
       <c r="A152" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="153" spans="1:1">
+      <c r="B152">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2">
       <c r="A153" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="154" spans="1:1">
+      <c r="B153">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2">
       <c r="A154" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="155" spans="1:1">
+      <c r="B154">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2">
       <c r="A155" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="156" spans="1:1">
+      <c r="B155">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2">
       <c r="A156" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="157" spans="1:1">
+      <c r="B156">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2">
       <c r="A157" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="158" spans="1:1">
+      <c r="B157">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2">
       <c r="A158" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="159" spans="1:1">
+      <c r="B158">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2">
       <c r="A159" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="160" spans="1:1">
+      <c r="B159">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2">
       <c r="A160" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="161" spans="1:1">
+      <c r="B160">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2">
       <c r="A161" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="162" spans="1:1">
+      <c r="B161">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2">
       <c r="A162" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="163" spans="1:1">
+      <c r="B162">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2">
       <c r="A163" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="164" spans="1:1">
+      <c r="B163">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2">
       <c r="A164" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="165" spans="1:1">
+      <c r="B164">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2">
       <c r="A165" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="166" spans="1:1">
+      <c r="B165">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2">
       <c r="A166" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="167" spans="1:1">
+      <c r="B166">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2">
       <c r="A167" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="168" spans="1:1">
+      <c r="B167">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2">
       <c r="A168" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="169" spans="1:1">
+      <c r="B168">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2">
       <c r="A169" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="170" spans="1:1">
+      <c r="B169">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2">
       <c r="A170" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="171" spans="1:1">
+      <c r="B170">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2">
       <c r="A171" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="172" spans="1:1">
+      <c r="B171">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2">
       <c r="A172" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="173" spans="1:1">
+      <c r="B172">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2">
       <c r="A173" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="174" spans="1:1">
+      <c r="B173">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2">
       <c r="A174" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="175" spans="1:1">
+      <c r="B174">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2">
       <c r="A175" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="176" spans="1:1">
+      <c r="B175">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2">
       <c r="A176" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="177" spans="1:1">
+      <c r="B176">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2">
       <c r="A177" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="178" spans="1:1">
+      <c r="B177">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2">
       <c r="A178" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="179" spans="1:1">
+      <c r="B178">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2">
       <c r="A179" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="180" spans="1:1">
+      <c r="B179">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2">
       <c r="A180" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="181" spans="1:1">
+      <c r="B180">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2">
       <c r="A181" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="182" spans="1:1">
+      <c r="B181">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2">
       <c r="A182" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="183" spans="1:1">
+      <c r="B182">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2">
       <c r="A183" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="184" spans="1:1">
+      <c r="B183">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2">
       <c r="A184" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="185" spans="1:1">
+      <c r="B184">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2">
       <c r="A185" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="186" spans="1:1">
+      <c r="B185">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2">
       <c r="A186" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="187" spans="1:1">
+      <c r="B186">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2">
       <c r="A187" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="188" spans="1:1">
+      <c r="B187">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2">
       <c r="A188" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="189" spans="1:1">
+      <c r="B188">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2">
       <c r="A189" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="190" spans="1:1">
+      <c r="B189">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2">
       <c r="A190" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="191" spans="1:1">
+      <c r="B190">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2">
       <c r="A191" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="192" spans="1:1">
+      <c r="B191">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2">
       <c r="A192" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="193" spans="1:1">
+      <c r="B192">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2">
       <c r="A193" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="194" spans="1:1">
+      <c r="B193">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2">
       <c r="A194" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="195" spans="1:1">
+      <c r="B194">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2">
       <c r="A195" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="196" spans="1:1">
+      <c r="B195">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2">
       <c r="A196" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="197" spans="1:1">
+      <c r="B196">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2">
       <c r="A197" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="198" spans="1:1">
+      <c r="B197">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2">
       <c r="A198" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="199" spans="1:1">
+      <c r="B198">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2">
       <c r="A199" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="200" spans="1:1">
+      <c r="B199">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2">
       <c r="A200" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="201" spans="1:1">
+      <c r="B200">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2">
       <c r="A201" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="202" spans="1:1">
+      <c r="B201">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2">
       <c r="A202" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="203" spans="1:1">
+      <c r="B202">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2">
       <c r="A203" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="204" spans="1:1">
+      <c r="B203">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2">
       <c r="A204" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="205" spans="1:1">
+      <c r="B204">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2">
       <c r="A205" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="206" spans="1:1">
+      <c r="B205">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2">
       <c r="A206" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="207" spans="1:1">
+      <c r="B206">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2">
       <c r="A207" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="208" spans="1:1">
+      <c r="B207">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2">
       <c r="A208" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="209" spans="1:1">
+      <c r="B208">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2">
       <c r="A209" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="210" spans="1:1">
+      <c r="B209">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2">
       <c r="A210" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="211" spans="1:1">
+      <c r="B210">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2">
       <c r="A211" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="212" spans="1:1">
+      <c r="B211">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2">
       <c r="A212" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="213" spans="1:1">
+      <c r="B212">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2">
       <c r="A213" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="214" spans="1:1">
+      <c r="B213">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2">
       <c r="A214" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="215" spans="1:1">
+      <c r="B214">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2">
       <c r="A215" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="216" spans="1:1">
+      <c r="B215">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2">
       <c r="A216" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="217" spans="1:1">
+      <c r="B216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2">
       <c r="A217" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="218" spans="1:1">
+      <c r="B217">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2">
       <c r="A218" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="219" spans="1:1">
+      <c r="B218">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2">
       <c r="A219" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="220" spans="1:1">
+      <c r="B219">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2">
       <c r="A220" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="221" spans="1:1">
+      <c r="B220">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2">
       <c r="A221" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="222" spans="1:1">
+      <c r="B221">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2">
       <c r="A222" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="223" spans="1:1">
+      <c r="B222">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2">
       <c r="A223" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="224" spans="1:1">
+      <c r="B223">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2">
       <c r="A224" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="225" spans="1:1">
+      <c r="B224">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2">
       <c r="A225" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="226" spans="1:1">
+      <c r="B225">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2">
       <c r="A226" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="227" spans="1:1">
+      <c r="B226">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2">
       <c r="A227" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="228" spans="1:1">
+      <c r="B227">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2">
       <c r="A228" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="229" spans="1:1">
+      <c r="B228">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2">
       <c r="A229" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="230" spans="1:1">
+      <c r="B229">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2">
       <c r="A230" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="231" spans="1:1">
+      <c r="B230">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2">
       <c r="A231" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="232" spans="1:1">
+      <c r="B231">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2">
       <c r="A232" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="233" spans="1:1">
+      <c r="B232">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2">
       <c r="A233" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="234" spans="1:1">
+      <c r="B233">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2">
       <c r="A234" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="235" spans="1:1">
+      <c r="B234">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2">
       <c r="A235" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="236" spans="1:1">
+      <c r="B235">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2">
       <c r="A236" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="237" spans="1:1">
+      <c r="B236">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2">
       <c r="A237" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="238" spans="1:1">
+      <c r="B237">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2">
       <c r="A238" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="239" spans="1:1">
+      <c r="B238">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2">
       <c r="A239" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="240" spans="1:1">
+      <c r="B239">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2">
       <c r="A240" t="s">
         <v>239</v>
+      </c>
+      <c r="B240">
+        <v>0</v>
       </c>
     </row>
     <row r="241" spans="1:2">
       <c r="A241" t="s">
         <v>240</v>
       </c>
+      <c r="B241">
+        <v>1</v>
+      </c>
     </row>
     <row r="242" spans="1:2">
       <c r="A242" t="s">
         <v>241</v>
       </c>
+      <c r="B242">
+        <v>1</v>
+      </c>
     </row>
     <row r="243" spans="1:2">
       <c r="A243" t="s">
         <v>242</v>
       </c>
+      <c r="B243">
+        <v>0</v>
+      </c>
     </row>
     <row r="244" spans="1:2">
       <c r="A244" t="s">
         <v>243</v>
       </c>
+      <c r="B244">
+        <v>0</v>
+      </c>
     </row>
     <row r="245" spans="1:2">
       <c r="A245" t="s">
         <v>244</v>
       </c>
+      <c r="B245">
+        <v>0</v>
+      </c>
     </row>
     <row r="246" spans="1:2">
       <c r="A246" t="s">
         <v>245</v>
       </c>
+      <c r="B246">
+        <v>0</v>
+      </c>
     </row>
     <row r="247" spans="1:2">
       <c r="A247" t="s">
         <v>246</v>
       </c>
+      <c r="B247">
+        <v>1</v>
+      </c>
     </row>
     <row r="248" spans="1:2">
       <c r="A248" t="s">
         <v>247</v>
       </c>
+      <c r="B248">
+        <v>0</v>
+      </c>
     </row>
     <row r="249" spans="1:2">
       <c r="A249" t="s">
         <v>248</v>
       </c>
+      <c r="B249">
+        <v>0</v>
+      </c>
     </row>
     <row r="250" spans="1:2">
       <c r="A250" t="s">
         <v>249</v>
       </c>
+      <c r="B250">
+        <v>0</v>
+      </c>
     </row>
     <row r="251" spans="1:2">
       <c r="A251" t="s">
         <v>250</v>
       </c>
+      <c r="B251">
+        <v>1</v>
+      </c>
     </row>
     <row r="252" spans="1:2">
       <c r="A252" t="s">
@@ -3708,7 +4455,7 @@
         <v>279</v>
       </c>
       <c r="B280">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="281" spans="1:2">
@@ -3783,7 +4530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="290" spans="1:2" ht="15">
+    <row r="290" spans="1:2">
       <c r="A290" s="2" t="s">
         <v>289</v>
       </c>
@@ -3807,7 +4554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="293" spans="1:2" ht="15">
+    <row r="293" spans="1:2">
       <c r="A293" s="2" t="s">
         <v>292</v>
       </c>
@@ -3894,13 +4641,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E201"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="13.75" customWidth="1"/>
+    <col min="2" max="2" width="13.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -5519,6 +6266,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C3E9AF5A3A25204D946F822282C6A3FA" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="10847e6e73796df1c5199be7b9d9bbac">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="760d57ad-6986-40cd-8f44-ffd131bfd400" xmlns:ns4="f201cd4c-f14b-4b50-a959-57fff54ecbfb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="472fd269b72ff4a8b63318727dbe4b51" ns3:_="" ns4:_="">
     <xsd:import namespace="760d57ad-6986-40cd-8f44-ffd131bfd400"/>
@@ -5703,22 +6465,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74C81C81-D3B0-4785-8AEB-71C808FAD019}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="760d57ad-6986-40cd-8f44-ffd131bfd400"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="f201cd4c-f14b-4b50-a959-57fff54ecbfb"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D5B91BB-EA3D-4631-B192-ED1BCC344988}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{42369E42-EB33-4F40-8133-C30C1A69E39F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5735,29 +6507,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D5B91BB-EA3D-4631-B192-ED1BCC344988}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74C81C81-D3B0-4785-8AEB-71C808FAD019}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="760d57ad-6986-40cd-8f44-ffd131bfd400"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="f201cd4c-f14b-4b50-a959-57fff54ecbfb"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>